<commit_message>
fixed an apparent typo with the first time box on the far right
</commit_message>
<xml_diff>
--- a/Docs/Schedule_Week3.xlsx
+++ b/Docs/Schedule_Week3.xlsx
@@ -113,9 +113,6 @@
     <t>Mandatory</t>
   </si>
   <si>
-    <t>10:00-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Room 308
 - Status Report/Demo
 (9:30AM)
@@ -136,6 +133,9 @@
     <t>EhPod/Meeting Room
 - Team meeting
 (10:30AM)</t>
+  </si>
+  <si>
+    <t>9:00-10:00</t>
   </si>
 </sst>
 </file>
@@ -143,16 +143,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="10">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.00%_);[Red]\(0.00%\)"/>
-    <numFmt numFmtId="170" formatCode="0%_);[Red]\(0%\)"/>
-    <numFmt numFmtId="171" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0.00%_);[Red]\(0.00%\)"/>
+    <numFmt numFmtId="169" formatCode="0%_);[Red]\(0%\)"/>
+    <numFmt numFmtId="170" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
   <fonts count="37" x14ac:knownFonts="1">
     <font>
@@ -975,7 +975,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2">
+    <xf numFmtId="5" fontId="8" fillId="0" borderId="2">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyBorder="0">
@@ -984,19 +984,19 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="5" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5"/>
     <xf numFmtId="4" fontId="8" fillId="20" borderId="5">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="8" fillId="21" borderId="5"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="6"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="6"/>
     <xf numFmtId="37" fontId="12" fillId="22" borderId="2" applyBorder="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1021,9 +1021,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="10"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="10"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="12"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="12"/>
     <xf numFmtId="0" fontId="32" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="0">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -1034,8 +1034,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="18" fillId="25" borderId="16"/>
-    <xf numFmtId="169" fontId="18" fillId="0" borderId="16" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="18" fillId="25" borderId="16"/>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="16" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0">
@@ -1049,8 +1049,8 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
@@ -1089,7 +1089,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="16" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="170" fontId="1" fillId="16" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
@@ -1865,8 +1865,8 @@
   </sheetPr>
   <dimension ref="B3:N18"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="D10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="11" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="12" t="s">
@@ -2014,20 +2014,20 @@
     </row>
     <row r="12" spans="2:11" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B12" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
       <c r="F12" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
       <c r="J12" s="24"/>
       <c r="K12" s="29" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -2036,14 +2036,14 @@
       <c r="D13" s="25"/>
       <c r="E13" s="22"/>
       <c r="F13" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="38" t="s">
         <v>23</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>24</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="19" t="s">

</xml_diff>

<commit_message>
-Reverted schedule to previous version. (not a typo - indicating times before 10:00am)
</commit_message>
<xml_diff>
--- a/Docs/Schedule_Week3.xlsx
+++ b/Docs/Schedule_Week3.xlsx
@@ -135,7 +135,7 @@
 (10:30AM)</t>
   </si>
   <si>
-    <t>9:00-10:00</t>
+    <t>-10:00</t>
   </si>
 </sst>
 </file>
@@ -143,16 +143,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="10">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.00%_);[Red]\(0.00%\)"/>
-    <numFmt numFmtId="169" formatCode="0%_);[Red]\(0%\)"/>
-    <numFmt numFmtId="170" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.00%_);[Red]\(0.00%\)"/>
+    <numFmt numFmtId="170" formatCode="0%_);[Red]\(0%\)"/>
+    <numFmt numFmtId="171" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
   <fonts count="37" x14ac:knownFonts="1">
     <font>
@@ -975,7 +975,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="5" fontId="8" fillId="0" borderId="2">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyBorder="0">
@@ -984,19 +984,19 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="5" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5"/>
     <xf numFmtId="4" fontId="8" fillId="20" borderId="5">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="8" fillId="21" borderId="5"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="6"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="6"/>
     <xf numFmtId="37" fontId="12" fillId="22" borderId="2" applyBorder="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1021,9 +1021,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="10"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="10"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="12"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="12"/>
     <xf numFmtId="0" fontId="32" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="0">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -1034,8 +1034,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="18" fillId="25" borderId="16"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="16" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="170" fontId="18" fillId="25" borderId="16"/>
+    <xf numFmtId="169" fontId="18" fillId="0" borderId="16" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0">
@@ -1049,8 +1049,8 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
@@ -1089,7 +1089,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="16" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="171" fontId="1" fillId="16" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
@@ -1865,8 +1865,8 @@
   </sheetPr>
   <dimension ref="B3:N18"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="D10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>